<commit_message>
Compil avec ajouts étapes, ref #38
</commit_message>
<xml_diff>
--- a/excel/repas.xlsx
+++ b/excel/repas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE90291-2931-D74B-A8C2-F0E6C7FADC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3761AEF-0B43-DC4B-953C-3486456BD3E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="560" windowWidth="34040" windowHeight="28180" activeTab="3" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
+    <workbookView xWindow="29900" yWindow="500" windowWidth="34040" windowHeight="28180" activeTab="3" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
   <sheets>
     <sheet name="DEJEUNER" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
   <si>
     <t>code</t>
   </si>
@@ -194,18 +194,6 @@
     <t>Dessert</t>
   </si>
   <si>
-    <t>Jus en fontaine</t>
-  </si>
-  <si>
-    <t>Fountain juice</t>
-  </si>
-  <si>
-    <t>Pain / Rôties</t>
-  </si>
-  <si>
-    <t>Bread /Toast</t>
-  </si>
-  <si>
     <t>Thé et café</t>
   </si>
   <si>
@@ -243,6 +231,12 @@
   </si>
   <si>
     <t>**Lunch box - 10h**&lt;br/&gt; Cold meat wrap, raw vegetables dip, cheese, orzo and Indian chickpea salad, biscuit, 200ml juice</t>
+  </si>
+  <si>
+    <t>Rôties</t>
+  </si>
+  <si>
+    <t>Toast</t>
   </si>
 </sst>
 </file>
@@ -312,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -338,15 +332,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -368,7 +358,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Bureau">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -406,7 +396,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Bureau">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -512,7 +502,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Bureau">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -838,10 +828,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -1036,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7675F6D-E77C-884B-B4A2-C26402FFC2F4}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1051,220 +1041,193 @@
     <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="F1" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" s="15" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="10">
+        <v>1</v>
+      </c>
+      <c r="D2" s="10">
+        <v>1</v>
+      </c>
+      <c r="E2" s="10">
+        <v>1</v>
+      </c>
+      <c r="F2" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="10">
+        <v>1</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
+      <c r="E3" s="10">
+        <v>1</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="10">
+        <v>1</v>
+      </c>
+      <c r="F4" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="10">
+        <v>1</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="10">
+        <v>1</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1</v>
+      </c>
+      <c r="E6" s="10">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="B8" s="9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="12">
-        <v>1</v>
-      </c>
-      <c r="D2" s="12">
-        <v>1</v>
-      </c>
-      <c r="E2" s="12">
-        <v>1</v>
-      </c>
-      <c r="F2" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="12">
-        <v>1</v>
-      </c>
-      <c r="D3" s="12">
-        <v>1</v>
-      </c>
-      <c r="E3" s="12">
-        <v>1</v>
-      </c>
-      <c r="F3" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="12">
-        <v>1</v>
-      </c>
-      <c r="F4" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="12">
-        <v>1</v>
-      </c>
-      <c r="D5" s="12">
-        <v>1</v>
-      </c>
-      <c r="E5" s="12">
-        <v>1</v>
-      </c>
-      <c r="F5" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="12">
-        <v>1</v>
-      </c>
-      <c r="D6" s="12">
-        <v>1</v>
-      </c>
-      <c r="E6" s="12">
-        <v>1</v>
-      </c>
-      <c r="F6" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="12">
-        <v>1</v>
-      </c>
-      <c r="F7" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="C8" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="28" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="28" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
+      <c r="E9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correction boite a lunch
</commit_message>
<xml_diff>
--- a/excel/repas.xlsx
+++ b/excel/repas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3761AEF-0B43-DC4B-953C-3486456BD3E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B614D2-59DF-044D-94BB-82C32FB783B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29900" yWindow="500" windowWidth="34040" windowHeight="28180" activeTab="3" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
+    <workbookView xWindow="29900" yWindow="500" windowWidth="34040" windowHeight="28180" activeTab="1" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
   <sheets>
     <sheet name="DEJEUNER" sheetId="4" r:id="rId1"/>
@@ -95,9 +95,6 @@
     <t>Soupe/potage, pain, salade repas au poulet grillé ou tacos, salade de fruits ou brownie, breuvage (jus, café, lait)</t>
   </si>
   <si>
-    <t>Soupe/potage, pain, lasagne italienne, salade césar, carré aux fraises, breuvage (jus, café, lait)</t>
-  </si>
-  <si>
     <t>Soup, bread, chicken fajitas, grilled vegetables, vegetable rice, green salad, apple crisp drink (juice, coffee, milk)</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>Soup, bread, grilled chicken meal salad or tacos, fruit salad or brownie, beverage (juice, coffee, milk)</t>
   </si>
   <si>
-    <t>Soup, bread, Italian lasagna, Caesar salad, strawberry square, beverage (juice, coffee, milk)</t>
-  </si>
-  <si>
     <t>Dim_Av</t>
   </si>
   <si>
@@ -237,6 +231,12 @@
   </si>
   <si>
     <t>Toast</t>
+  </si>
+  <si>
+    <t>**Boîte à lunch - xxh**&lt;br/&gt; TBD</t>
+  </si>
+  <si>
+    <t>**Lunch box - xxh**&lt;br/&gt; TBD</t>
   </si>
 </sst>
 </file>
@@ -750,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C23D3F-FE64-A34F-B126-68B68B58113C}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -783,7 +783,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="5"/>
     </row>
@@ -795,7 +795,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -807,7 +807,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -819,7 +819,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="5"/>
     </row>
@@ -828,10 +828,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -843,7 +843,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="5"/>
     </row>
@@ -852,10 +852,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="D8" s="6"/>
     </row>
@@ -912,13 +912,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2" s="4"/>
     </row>
@@ -927,10 +927,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D3" s="5"/>
     </row>
@@ -939,10 +939,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -954,7 +954,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -963,10 +963,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -975,10 +975,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D7" s="5"/>
     </row>
@@ -987,10 +987,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D8" s="5"/>
     </row>
@@ -999,10 +999,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" s="6"/>
     </row>
@@ -1028,7 +1028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7675F6D-E77C-884B-B4A2-C26402FFC2F4}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -1043,30 +1043,30 @@
   <sheetData>
     <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="11" t="s">
+      <c r="E1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>59</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" s="10">
         <v>1</v>
@@ -1083,10 +1083,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" s="10">
         <v>1</v>
@@ -1103,16 +1103,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4" s="10">
         <v>1</v>
@@ -1123,10 +1123,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C5" s="10">
         <v>1</v>
@@ -1143,10 +1143,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" s="10">
         <v>1</v>
@@ -1163,16 +1163,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E7" s="10">
         <v>1</v>
@@ -1183,42 +1183,42 @@
     </row>
     <row r="8" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>54</v>
-      </c>
       <c r="D9" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>